<commit_message>
Main game, draw animated gifs
</commit_message>
<xml_diff>
--- a/players/players.xlsx
+++ b/players/players.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edsmilde/scratch/roadrace/players/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edsmilde/w/roadrace/players/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A227EA00-453B-F847-824D-F09311A495BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B572B1-F9DE-164B-AB70-7E332DEDE600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="600" windowWidth="28040" windowHeight="16180" xr2:uid="{94C6DEA4-89FB-7E43-AF13-99FC7CAAED3F}"/>
+    <workbookView xWindow="980" yWindow="600" windowWidth="28040" windowHeight="16180" xr2:uid="{94C6DEA4-89FB-7E43-AF13-99FC7CAAED3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="216">
   <si>
     <t>FirstName</t>
   </si>
@@ -288,12 +288,6 @@
     <t>BR</t>
   </si>
   <si>
-    <t>Gilmar Silvestre</t>
-  </si>
-  <si>
-    <t>Lopes</t>
-  </si>
-  <si>
     <t>Jared</t>
   </si>
   <si>
@@ -622,13 +616,70 @@
   </si>
   <si>
     <t>Linkletter</t>
+  </si>
+  <si>
+    <t>StartEnergy</t>
+  </si>
+  <si>
+    <t>ImpatienceFactor</t>
+  </si>
+  <si>
+    <t>FieldA</t>
+  </si>
+  <si>
+    <t>FieldB</t>
+  </si>
+  <si>
+    <t>FieldC</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>FieldOlympics</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Do Nascimento</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>Ringer</t>
+  </si>
+  <si>
+    <t>Othmane</t>
+  </si>
+  <si>
+    <t>El Gourmi</t>
+  </si>
+  <si>
+    <t>Gilmar</t>
+  </si>
+  <si>
+    <t>Silvestre Lopes</t>
+  </si>
+  <si>
+    <t>asics</t>
+  </si>
+  <si>
+    <t>adidas white</t>
+  </si>
+  <si>
+    <t>saucony blue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -973,13 +1024,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4587E4C2-CE81-0443-B7FE-A4DBB4F33474}">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
@@ -993,7 +1044,7 @@
     <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1024,16 +1075,37 @@
       <c r="J1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M1" t="s">
+        <v>199</v>
+      </c>
+      <c r="N1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>140</v>
-      </c>
-      <c r="B2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D2" t="s">
-        <v>142</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1048,18 +1120,39 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>177</v>
+      </c>
+      <c r="J2">
+        <v>69</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N2" t="s">
+        <v>202</v>
+      </c>
+      <c r="O2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1074,18 +1167,39 @@
         <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>177</v>
+      </c>
+      <c r="J3">
+        <v>69</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>202</v>
+      </c>
+      <c r="N3" t="s">
+        <v>202</v>
+      </c>
+      <c r="O3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1100,18 +1214,42 @@
         <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>177</v>
+      </c>
+      <c r="J4">
+        <v>69</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>202</v>
+      </c>
+      <c r="N4" t="s">
+        <v>202</v>
+      </c>
+      <c r="O4" t="s">
+        <v>202</v>
+      </c>
+      <c r="P4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1126,16 +1264,40 @@
         <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>177</v>
+      </c>
+      <c r="J5">
+        <v>69</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>202</v>
+      </c>
+      <c r="N5" t="s">
+        <v>202</v>
+      </c>
+      <c r="O5" t="s">
+        <v>202</v>
+      </c>
+      <c r="P5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" t="s">
         <v>66</v>
       </c>
@@ -1154,14 +1316,38 @@
       <c r="I6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6">
+        <v>70</v>
+      </c>
+      <c r="K6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>202</v>
+      </c>
+      <c r="N6" t="s">
+        <v>202</v>
+      </c>
+      <c r="O6" t="s">
+        <v>202</v>
+      </c>
+      <c r="P6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>56</v>
       </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
       <c r="D7" t="s">
         <v>66</v>
       </c>
@@ -1178,16 +1364,40 @@
         <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>177</v>
+      </c>
+      <c r="J7">
+        <v>72</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>202</v>
+      </c>
+      <c r="N7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O7" t="s">
+        <v>202</v>
+      </c>
+      <c r="P7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>85</v>
       </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
       <c r="D8" t="s">
         <v>86</v>
       </c>
@@ -1201,18 +1411,39 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="J8">
+        <v>69</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>202</v>
+      </c>
+      <c r="N8" t="s">
+        <v>202</v>
+      </c>
+      <c r="O8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>212</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>86</v>
@@ -1227,59 +1458,101 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="J9">
+        <v>69</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>202</v>
+      </c>
+      <c r="N9" t="s">
+        <v>202</v>
+      </c>
+      <c r="O9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>176</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10">
+        <v>69</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>202</v>
+      </c>
+      <c r="N10" t="s">
+        <v>202</v>
+      </c>
+      <c r="O10" t="s">
+        <v>202</v>
+      </c>
+      <c r="P10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>0.9</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
       <c r="G11">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
         <v>11</v>
@@ -1287,16 +1560,37 @@
       <c r="I11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11">
+        <v>69</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>202</v>
+      </c>
+      <c r="N11" t="s">
+        <v>202</v>
+      </c>
+      <c r="O11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>214</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1305,50 +1599,92 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H12" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12">
+        <v>69</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>202</v>
+      </c>
+      <c r="N12" t="s">
+        <v>202</v>
+      </c>
+      <c r="O12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>176</v>
+      </c>
+      <c r="I13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
+      <c r="J13">
+        <v>69</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>202</v>
+      </c>
+      <c r="N13" t="s">
+        <v>202</v>
+      </c>
+      <c r="O13" t="s">
+        <v>202</v>
+      </c>
+      <c r="P13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
       </c>
       <c r="D14" t="s">
         <v>64</v>
@@ -1363,157 +1699,280 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" t="s">
+        <v>177</v>
+      </c>
+      <c r="J14">
+        <v>69</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>202</v>
+      </c>
+      <c r="N14" t="s">
+        <v>202</v>
+      </c>
+      <c r="O14" t="s">
+        <v>202</v>
+      </c>
+      <c r="P14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
         <v>16</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
+      <c r="J15">
+        <v>69</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>202</v>
+      </c>
+      <c r="N15" t="s">
+        <v>202</v>
+      </c>
+      <c r="O15" t="s">
+        <v>202</v>
+      </c>
+      <c r="P15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="D15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="C16" t="s">
+        <v>214</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>29</v>
       </c>
-      <c r="I15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
+      <c r="I16" t="s">
+        <v>177</v>
+      </c>
+      <c r="J16">
+        <v>69</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>202</v>
+      </c>
+      <c r="N16" t="s">
+        <v>202</v>
+      </c>
+      <c r="O16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" t="s">
+        <v>177</v>
+      </c>
+      <c r="J17">
+        <v>69</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>202</v>
+      </c>
+      <c r="N17" t="s">
+        <v>202</v>
+      </c>
+      <c r="O17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>57</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>178</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>176</v>
+      </c>
+      <c r="I18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="J18">
+        <v>69</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>202</v>
+      </c>
+      <c r="N18" t="s">
+        <v>202</v>
+      </c>
+      <c r="O18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
         <v>68</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>176</v>
+      </c>
+      <c r="I19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" t="s">
+      <c r="J19">
+        <v>69</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>202</v>
+      </c>
+      <c r="N19" t="s">
+        <v>202</v>
+      </c>
+      <c r="O19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0.9</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" t="s">
-        <v>131</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -1522,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1536,13 +1995,31 @@
       <c r="J20">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
+        <v>202</v>
+      </c>
+      <c r="N20" t="s">
+        <v>202</v>
+      </c>
+      <c r="O20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>133</v>
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>214</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -1551,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1563,24 +2040,42 @@
         <v>18</v>
       </c>
       <c r="J21">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>64</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21" t="s">
+        <v>202</v>
+      </c>
+      <c r="N21" t="s">
+        <v>202</v>
+      </c>
+      <c r="O21" t="s">
+        <v>202</v>
+      </c>
+      <c r="P21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>214</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0.9</v>
@@ -1589,76 +2084,139 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J22">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>64</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>202</v>
+      </c>
+      <c r="N22" t="s">
+        <v>202</v>
+      </c>
+      <c r="O22" t="s">
+        <v>202</v>
+      </c>
+      <c r="P22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>131</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>18</v>
+      </c>
+      <c r="J23">
+        <v>73</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>202</v>
+      </c>
+      <c r="N23" t="s">
+        <v>202</v>
+      </c>
+      <c r="O23" t="s">
+        <v>202</v>
+      </c>
+      <c r="P23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G24">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="I24" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>12</v>
+      </c>
+      <c r="J24">
+        <v>69</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>202</v>
+      </c>
+      <c r="N24" t="s">
+        <v>202</v>
+      </c>
+      <c r="O24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
@@ -1670,21 +2228,45 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
       </c>
       <c r="I25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>177</v>
+      </c>
+      <c r="J25">
+        <v>69</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
+        <v>202</v>
+      </c>
+      <c r="N25" t="s">
+        <v>202</v>
+      </c>
+      <c r="O25" t="s">
+        <v>202</v>
+      </c>
+      <c r="P25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="C26" t="s">
+        <v>161</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
@@ -1702,15 +2284,36 @@
         <v>29</v>
       </c>
       <c r="I26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>177</v>
+      </c>
+      <c r="J26">
+        <v>69</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>202</v>
+      </c>
+      <c r="N26" t="s">
+        <v>202</v>
+      </c>
+      <c r="O26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>178</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>122</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
       </c>
       <c r="D27" t="s">
         <v>26</v>
@@ -1722,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H27" t="s">
         <v>29</v>
@@ -1730,16 +2333,34 @@
       <c r="I27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="J27">
+        <v>69</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>202</v>
+      </c>
+      <c r="N27" t="s">
+        <v>202</v>
+      </c>
+      <c r="O27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="C28" t="s">
-        <v>158</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
         <v>26</v>
@@ -1751,73 +2372,139 @@
         <v>1</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H28" t="s">
         <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>30</v>
+      </c>
+      <c r="J28">
+        <v>69</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>202</v>
+      </c>
+      <c r="N28" t="s">
+        <v>202</v>
+      </c>
+      <c r="O28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1.2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29">
+        <v>69</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29" t="s">
+        <v>202</v>
+      </c>
+      <c r="N29" t="s">
+        <v>202</v>
+      </c>
+      <c r="O29" t="s">
+        <v>202</v>
+      </c>
+      <c r="P29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" t="s">
+        <v>177</v>
+      </c>
+      <c r="J30">
+        <v>69</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30" t="s">
+        <v>202</v>
+      </c>
+      <c r="N30" t="s">
+        <v>202</v>
+      </c>
+      <c r="O30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>70</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>71</v>
       </c>
-      <c r="D29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>178</v>
-      </c>
-      <c r="I29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30" t="s">
-        <v>178</v>
-      </c>
-      <c r="I30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
+      <c r="C31" t="s">
+        <v>25</v>
       </c>
       <c r="D31" t="s">
         <v>81</v>
@@ -1832,79 +2519,142 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="J31">
+        <v>69</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
+        <v>202</v>
+      </c>
+      <c r="N31" t="s">
+        <v>202</v>
+      </c>
+      <c r="O31" t="s">
+        <v>202</v>
+      </c>
+      <c r="P31" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>213</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>176</v>
+      </c>
+      <c r="I32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32">
+        <v>69</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
+        <v>202</v>
+      </c>
+      <c r="N32" t="s">
+        <v>202</v>
+      </c>
+      <c r="O32" t="s">
+        <v>202</v>
+      </c>
+      <c r="P32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>176</v>
+      </c>
+      <c r="I33" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33">
+        <v>69</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33" t="s">
+        <v>202</v>
+      </c>
+      <c r="N33" t="s">
+        <v>202</v>
+      </c>
+      <c r="O33" t="s">
+        <v>202</v>
+      </c>
+      <c r="P33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>7</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>8</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>9</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0.9</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="H32" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0.9</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -1924,13 +2674,37 @@
       <c r="I34" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34">
+        <v>67</v>
+      </c>
+      <c r="K34">
+        <v>1.2</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34" t="s">
+        <v>202</v>
+      </c>
+      <c r="N34" t="s">
+        <v>202</v>
+      </c>
+      <c r="O34" t="s">
+        <v>202</v>
+      </c>
+      <c r="P34" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -1942,7 +2716,7 @@
         <v>0.9</v>
       </c>
       <c r="G35">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H35" t="s">
         <v>11</v>
@@ -1950,16 +2724,40 @@
       <c r="I35" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35">
+        <v>69</v>
+      </c>
+      <c r="K35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35" t="s">
+        <v>202</v>
+      </c>
+      <c r="N35" t="s">
+        <v>202</v>
+      </c>
+      <c r="O35" t="s">
+        <v>202</v>
+      </c>
+      <c r="P35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
       </c>
       <c r="D36" t="s">
-        <v>156</v>
+        <v>10</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1971,200 +2769,386 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="I36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>12</v>
+      </c>
+      <c r="J36">
+        <v>69</v>
+      </c>
+      <c r="K36">
+        <v>1.2</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36" t="s">
+        <v>202</v>
+      </c>
+      <c r="N36" t="s">
+        <v>202</v>
+      </c>
+      <c r="O36" t="s">
+        <v>202</v>
+      </c>
+      <c r="P36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>133</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="I37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>12</v>
+      </c>
+      <c r="J37">
+        <v>69</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N37" t="s">
+        <v>202</v>
+      </c>
+      <c r="O37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>151</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I38" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38">
+        <v>74</v>
+      </c>
+      <c r="K38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38" t="s">
+        <v>202</v>
+      </c>
+      <c r="N38" t="s">
+        <v>202</v>
+      </c>
+      <c r="O38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>209</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>210</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
       </c>
       <c r="D39" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I39" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39">
+        <v>69</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" t="s">
+        <v>202</v>
+      </c>
+      <c r="N39" t="s">
+        <v>202</v>
+      </c>
+      <c r="O39" t="s">
+        <v>202</v>
+      </c>
+      <c r="P39" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>176</v>
+      </c>
+      <c r="I40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40">
+        <v>69</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40" t="s">
+        <v>202</v>
+      </c>
+      <c r="N40" t="s">
+        <v>202</v>
+      </c>
+      <c r="O40" t="s">
+        <v>202</v>
+      </c>
+      <c r="P40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>176</v>
+      </c>
+      <c r="I41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41">
+        <v>69</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41" t="s">
+        <v>202</v>
+      </c>
+      <c r="N41" t="s">
+        <v>202</v>
+      </c>
+      <c r="O41" t="s">
+        <v>202</v>
+      </c>
+      <c r="P41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>176</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42">
+        <v>69</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42" t="s">
+        <v>202</v>
+      </c>
+      <c r="N42" t="s">
+        <v>202</v>
+      </c>
+      <c r="O42" t="s">
+        <v>202</v>
+      </c>
+      <c r="P42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>31</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>54</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
         <v>67</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
         <v>0.9</v>
       </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
         <v>16</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I43" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
+      <c r="J43">
+        <v>65</v>
+      </c>
+      <c r="K43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43" t="s">
+        <v>202</v>
+      </c>
+      <c r="N43" t="s">
+        <v>202</v>
+      </c>
+      <c r="O43" t="s">
+        <v>202</v>
+      </c>
+      <c r="P43" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>51</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>52</v>
       </c>
-      <c r="D41" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41" t="s">
-        <v>29</v>
-      </c>
-      <c r="I41" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" t="s">
-        <v>119</v>
-      </c>
-      <c r="D42" t="s">
-        <v>65</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>1.2</v>
-      </c>
-      <c r="H42" t="s">
-        <v>29</v>
-      </c>
-      <c r="I42" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>120</v>
-      </c>
-      <c r="B43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>1.2</v>
-      </c>
-      <c r="H43" t="s">
-        <v>29</v>
-      </c>
-      <c r="I43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" t="s">
-        <v>119</v>
+      <c r="C44" t="s">
+        <v>21</v>
       </c>
       <c r="D44" t="s">
         <v>65</v>
@@ -2176,24 +3160,45 @@
         <v>1</v>
       </c>
       <c r="G44">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H44" t="s">
         <v>29</v>
       </c>
       <c r="I44" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>177</v>
+      </c>
+      <c r="J44">
+        <v>69</v>
+      </c>
+      <c r="K44">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44" t="s">
+        <v>202</v>
+      </c>
+      <c r="N44" t="s">
+        <v>202</v>
+      </c>
+      <c r="O44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>117</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -2202,24 +3207,45 @@
         <v>1</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="H45" t="s">
         <v>29</v>
       </c>
       <c r="I45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>177</v>
+      </c>
+      <c r="J45">
+        <v>72</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45" t="s">
+        <v>202</v>
+      </c>
+      <c r="N45" t="s">
+        <v>202</v>
+      </c>
+      <c r="O45" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
+        <v>117</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2228,7 +3254,7 @@
         <v>1</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="H46" t="s">
         <v>29</v>
@@ -2236,16 +3262,37 @@
       <c r="I46" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46">
+        <v>74</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46" t="s">
+        <v>202</v>
+      </c>
+      <c r="N46" t="s">
+        <v>202</v>
+      </c>
+      <c r="O46" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>117</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2254,198 +3301,333 @@
         <v>1</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="H47" t="s">
         <v>29</v>
       </c>
       <c r="I47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>177</v>
+      </c>
+      <c r="J47">
+        <v>71</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47" t="s">
+        <v>202</v>
+      </c>
+      <c r="N47" t="s">
+        <v>202</v>
+      </c>
+      <c r="O47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="I48" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>30</v>
+      </c>
+      <c r="J48">
+        <v>69</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48" t="s">
+        <v>202</v>
+      </c>
+      <c r="N48" t="s">
+        <v>202</v>
+      </c>
+      <c r="O48" t="s">
+        <v>202</v>
+      </c>
+      <c r="P48" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>136</v>
       </c>
       <c r="B49" t="s">
         <v>137</v>
       </c>
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
       <c r="D49" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G49">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I49" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+        <v>30</v>
+      </c>
+      <c r="J49">
+        <v>69</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49" t="s">
+        <v>202</v>
+      </c>
+      <c r="N49" t="s">
+        <v>202</v>
+      </c>
+      <c r="O49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="C50" t="s">
         <v>21</v>
       </c>
       <c r="D50" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>29</v>
+      </c>
+      <c r="I50" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50">
+        <v>69</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50" t="s">
+        <v>202</v>
+      </c>
+      <c r="N50" t="s">
+        <v>202</v>
+      </c>
+      <c r="O50" t="s">
+        <v>202</v>
+      </c>
+      <c r="P50" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
         <v>0.9</v>
       </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50" t="s">
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
         <v>11</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I51" t="s">
         <v>12</v>
       </c>
-      <c r="J50">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" t="s">
-        <v>28</v>
-      </c>
-      <c r="C51" t="s">
-        <v>25</v>
-      </c>
-      <c r="D51" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="H51" t="s">
-        <v>29</v>
-      </c>
-      <c r="I51" t="s">
-        <v>30</v>
-      </c>
       <c r="J51">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+        <v>69</v>
+      </c>
+      <c r="K51">
+        <v>1.2</v>
+      </c>
+      <c r="L51">
+        <v>1.5</v>
+      </c>
+      <c r="M51" t="s">
+        <v>202</v>
+      </c>
+      <c r="N51" t="s">
+        <v>202</v>
+      </c>
+      <c r="O51" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="C52" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G52">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H52" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="I52" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="J52">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+        <v>69</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52" t="s">
+        <v>202</v>
+      </c>
+      <c r="N52" t="s">
+        <v>202</v>
+      </c>
+      <c r="O52" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="C53" t="s">
+        <v>21</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G53">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I53" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="J53">
+        <v>71</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53" t="s">
+        <v>202</v>
+      </c>
+      <c r="N53" t="s">
+        <v>202</v>
+      </c>
+      <c r="O53" t="s">
+        <v>202</v>
+      </c>
+      <c r="P53" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
@@ -2463,15 +3645,39 @@
         <v>29</v>
       </c>
       <c r="I54" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>30</v>
+      </c>
+      <c r="J54">
+        <v>71</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54" t="s">
+        <v>202</v>
+      </c>
+      <c r="N54" t="s">
+        <v>202</v>
+      </c>
+      <c r="O54" t="s">
+        <v>202</v>
+      </c>
+      <c r="P54" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>33</v>
+      </c>
+      <c r="C55" t="s">
+        <v>34</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -2483,7 +3689,7 @@
         <v>1</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="H55" t="s">
         <v>29</v>
@@ -2491,13 +3697,37 @@
       <c r="I55" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="J55">
+        <v>73</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55" t="s">
+        <v>202</v>
+      </c>
+      <c r="N55" t="s">
+        <v>202</v>
+      </c>
+      <c r="O55" t="s">
+        <v>202</v>
+      </c>
+      <c r="P55" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>21</v>
       </c>
       <c r="D56" t="s">
         <v>22</v>
@@ -2509,21 +3739,42 @@
         <v>1</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H56" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I56" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>12</v>
+      </c>
+      <c r="J56">
+        <v>69</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56" t="s">
+        <v>202</v>
+      </c>
+      <c r="N56" t="s">
+        <v>202</v>
+      </c>
+      <c r="O56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>88</v>
+      </c>
+      <c r="C57" t="s">
+        <v>215</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -2532,24 +3783,45 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="I57" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+        <v>179</v>
+      </c>
+      <c r="J57">
+        <v>69</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57" t="s">
+        <v>202</v>
+      </c>
+      <c r="N57" t="s">
+        <v>202</v>
+      </c>
+      <c r="O57" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B58" t="s">
-        <v>100</v>
+        <v>92</v>
+      </c>
+      <c r="C58" t="s">
+        <v>215</v>
       </c>
       <c r="D58" t="s">
         <v>22</v>
@@ -2564,18 +3836,39 @@
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="I58" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>30</v>
+      </c>
+      <c r="J58">
+        <v>69</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58" t="s">
+        <v>202</v>
+      </c>
+      <c r="N58" t="s">
+        <v>202</v>
+      </c>
+      <c r="O58" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>21</v>
       </c>
       <c r="D59" t="s">
         <v>22</v>
@@ -2590,18 +3883,39 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="I59" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+        <v>18</v>
+      </c>
+      <c r="J59">
+        <v>69</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59" t="s">
+        <v>202</v>
+      </c>
+      <c r="N59" t="s">
+        <v>202</v>
+      </c>
+      <c r="O59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
-        <v>108</v>
+        <v>96</v>
+      </c>
+      <c r="C60" t="s">
+        <v>21</v>
       </c>
       <c r="D60" t="s">
         <v>22</v>
@@ -2610,27 +3924,45 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G60">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="I60" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <v>18</v>
+      </c>
+      <c r="J60">
+        <v>69</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+      <c r="M60" t="s">
+        <v>202</v>
+      </c>
+      <c r="N60" t="s">
+        <v>202</v>
+      </c>
+      <c r="O60" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
-        <v>171</v>
+        <v>21</v>
       </c>
       <c r="D61" t="s">
         <v>22</v>
@@ -2642,21 +3974,42 @@
         <v>1</v>
       </c>
       <c r="G61">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="I61" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+        <v>18</v>
+      </c>
+      <c r="J61">
+        <v>69</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
+      <c r="M61" t="s">
+        <v>202</v>
+      </c>
+      <c r="N61" t="s">
+        <v>202</v>
+      </c>
+      <c r="O61" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="C62" t="s">
+        <v>214</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -2674,18 +4027,36 @@
         <v>29</v>
       </c>
       <c r="I62" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+        <v>177</v>
+      </c>
+      <c r="J62">
+        <v>69</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="M62" t="s">
+        <v>202</v>
+      </c>
+      <c r="N62" t="s">
+        <v>202</v>
+      </c>
+      <c r="O62" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B63" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="D63" t="s">
         <v>22</v>
@@ -2697,24 +4068,42 @@
         <v>1</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="H63" t="s">
         <v>29</v>
       </c>
       <c r="I63" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+        <v>17</v>
+      </c>
+      <c r="J63">
+        <v>69</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+      <c r="M63" t="s">
+        <v>202</v>
+      </c>
+      <c r="N63" t="s">
+        <v>202</v>
+      </c>
+      <c r="O63" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D64" t="s">
         <v>22</v>
@@ -2726,24 +4115,42 @@
         <v>1</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="H64" t="s">
         <v>29</v>
       </c>
       <c r="I64" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>177</v>
+      </c>
+      <c r="J64">
+        <v>69</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64" t="s">
+        <v>202</v>
+      </c>
+      <c r="N64" t="s">
+        <v>202</v>
+      </c>
+      <c r="O64" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="D65" t="s">
         <v>22</v>
@@ -2758,21 +4165,39 @@
         <v>1</v>
       </c>
       <c r="H65" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I65" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>177</v>
+      </c>
+      <c r="J65">
+        <v>69</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65" t="s">
+        <v>202</v>
+      </c>
+      <c r="N65" t="s">
+        <v>202</v>
+      </c>
+      <c r="O65" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="B66" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="C66" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -2790,18 +4215,36 @@
         <v>29</v>
       </c>
       <c r="I66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>179</v>
+      </c>
+      <c r="J66">
+        <v>69</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66" t="s">
+        <v>202</v>
+      </c>
+      <c r="N66" t="s">
+        <v>202</v>
+      </c>
+      <c r="O66" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="C67" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
         <v>22</v>
@@ -2819,18 +4262,36 @@
         <v>29</v>
       </c>
       <c r="I67" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>30</v>
+      </c>
+      <c r="J67">
+        <v>69</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="M67" t="s">
+        <v>202</v>
+      </c>
+      <c r="N67" t="s">
+        <v>202</v>
+      </c>
+      <c r="O67" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B68" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="C68" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -2845,21 +4306,39 @@
         <v>1</v>
       </c>
       <c r="H68" t="s">
-        <v>29</v>
+        <v>176</v>
       </c>
       <c r="I68" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>18</v>
+      </c>
+      <c r="J68">
+        <v>69</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+      <c r="M68" t="s">
+        <v>202</v>
+      </c>
+      <c r="N68" t="s">
+        <v>202</v>
+      </c>
+      <c r="O68" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C69" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -2877,18 +4356,36 @@
         <v>29</v>
       </c>
       <c r="I69" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>30</v>
+      </c>
+      <c r="J69">
+        <v>69</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+      <c r="M69" t="s">
+        <v>202</v>
+      </c>
+      <c r="N69" t="s">
+        <v>202</v>
+      </c>
+      <c r="O69" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B70" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C70" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
@@ -2906,18 +4403,36 @@
         <v>29</v>
       </c>
       <c r="I70" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>17</v>
+      </c>
+      <c r="J70">
+        <v>69</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70" t="s">
+        <v>202</v>
+      </c>
+      <c r="N70" t="s">
+        <v>202</v>
+      </c>
+      <c r="O70" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="B71" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C71" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D71" t="s">
         <v>22</v>
@@ -2935,18 +4450,36 @@
         <v>29</v>
       </c>
       <c r="I71" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>30</v>
+      </c>
+      <c r="J71">
+        <v>69</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71" t="s">
+        <v>202</v>
+      </c>
+      <c r="N71" t="s">
+        <v>202</v>
+      </c>
+      <c r="O71" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D72" t="s">
         <v>22</v>
@@ -2964,18 +4497,36 @@
         <v>29</v>
       </c>
       <c r="I72" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+        <v>177</v>
+      </c>
+      <c r="J72">
+        <v>69</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="M72" t="s">
+        <v>202</v>
+      </c>
+      <c r="N72" t="s">
+        <v>202</v>
+      </c>
+      <c r="O72" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B73" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="C73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -2993,18 +4544,36 @@
         <v>29</v>
       </c>
       <c r="I73" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+        <v>177</v>
+      </c>
+      <c r="J73">
+        <v>69</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73" t="s">
+        <v>202</v>
+      </c>
+      <c r="N73" t="s">
+        <v>202</v>
+      </c>
+      <c r="O73" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C74" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D74" t="s">
         <v>22</v>
@@ -3013,33 +4582,51 @@
         <v>0</v>
       </c>
       <c r="F74">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G74">
         <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I74" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>17</v>
+      </c>
+      <c r="J74">
+        <v>69</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74" t="s">
+        <v>202</v>
+      </c>
+      <c r="N74" t="s">
+        <v>202</v>
+      </c>
+      <c r="O74" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B75" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C75" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D75" t="s">
         <v>22</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -3048,21 +4635,42 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="I75" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+        <v>30</v>
+      </c>
+      <c r="J75">
+        <v>69</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="M75" t="s">
+        <v>202</v>
+      </c>
+      <c r="N75" t="s">
+        <v>202</v>
+      </c>
+      <c r="O75" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B76" t="s">
-        <v>183</v>
+        <v>111</v>
+      </c>
+      <c r="C76" t="s">
+        <v>156</v>
       </c>
       <c r="D76" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -3074,50 +4682,92 @@
         <v>1</v>
       </c>
       <c r="H76" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I76" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+        <v>177</v>
+      </c>
+      <c r="J76">
+        <v>69</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>1</v>
+      </c>
+      <c r="M76" t="s">
+        <v>202</v>
+      </c>
+      <c r="N76" t="s">
+        <v>202</v>
+      </c>
+      <c r="O76" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B77" t="s">
-        <v>185</v>
+        <v>173</v>
+      </c>
+      <c r="C77" t="s">
+        <v>169</v>
       </c>
       <c r="D77" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G77">
         <v>1</v>
       </c>
       <c r="H77" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="I77" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77">
+        <v>69</v>
+      </c>
+      <c r="K77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77" t="s">
+        <v>202</v>
+      </c>
+      <c r="N77" t="s">
+        <v>202</v>
+      </c>
+      <c r="O77" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B78" t="s">
-        <v>187</v>
+        <v>175</v>
+      </c>
+      <c r="C78" t="s">
+        <v>21</v>
       </c>
       <c r="D78" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -3126,18 +4776,39 @@
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="I78" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+        <v>12</v>
+      </c>
+      <c r="J78">
+        <v>69</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+      <c r="M78" t="s">
+        <v>202</v>
+      </c>
+      <c r="N78" t="s">
+        <v>202</v>
+      </c>
+      <c r="O78" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B79" t="s">
-        <v>189</v>
+        <v>181</v>
+      </c>
+      <c r="C79" t="s">
+        <v>213</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -3152,18 +4823,39 @@
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I79" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79">
+        <v>69</v>
+      </c>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79" t="s">
+        <v>202</v>
+      </c>
+      <c r="N79" t="s">
+        <v>202</v>
+      </c>
+      <c r="O79" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B80" t="s">
-        <v>193</v>
+        <v>183</v>
+      </c>
+      <c r="C80" t="s">
+        <v>213</v>
       </c>
       <c r="D80" t="s">
         <v>81</v>
@@ -3178,18 +4870,39 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I80" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80">
+        <v>69</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80" t="s">
+        <v>202</v>
+      </c>
+      <c r="N80" t="s">
+        <v>202</v>
+      </c>
+      <c r="O80" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B81" t="s">
-        <v>191</v>
+        <v>185</v>
+      </c>
+      <c r="C81" t="s">
+        <v>213</v>
       </c>
       <c r="D81" t="s">
         <v>81</v>
@@ -3204,102 +4917,315 @@
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I81" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81">
+        <v>69</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81" t="s">
+        <v>202</v>
+      </c>
+      <c r="N81" t="s">
+        <v>202</v>
+      </c>
+      <c r="O81" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>186</v>
+      </c>
+      <c r="B82" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" t="s">
+        <v>213</v>
+      </c>
+      <c r="D82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82" t="s">
+        <v>176</v>
+      </c>
+      <c r="I82" t="s">
+        <v>18</v>
+      </c>
+      <c r="J82">
+        <v>69</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+      <c r="M82" t="s">
+        <v>202</v>
+      </c>
+      <c r="N82" t="s">
+        <v>202</v>
+      </c>
+      <c r="O82" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>190</v>
+      </c>
+      <c r="B83" t="s">
+        <v>191</v>
+      </c>
+      <c r="C83" t="s">
+        <v>213</v>
+      </c>
+      <c r="D83" t="s">
+        <v>81</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83" t="s">
+        <v>176</v>
+      </c>
+      <c r="I83" t="s">
+        <v>18</v>
+      </c>
+      <c r="J83">
+        <v>69</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83" t="s">
+        <v>202</v>
+      </c>
+      <c r="N83" t="s">
+        <v>202</v>
+      </c>
+      <c r="O83" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" t="s">
+        <v>189</v>
+      </c>
+      <c r="C84" t="s">
+        <v>213</v>
+      </c>
+      <c r="D84" t="s">
+        <v>81</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84" t="s">
+        <v>176</v>
+      </c>
+      <c r="I84" t="s">
+        <v>18</v>
+      </c>
+      <c r="J84">
+        <v>69</v>
+      </c>
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="M84" t="s">
+        <v>202</v>
+      </c>
+      <c r="N84" t="s">
+        <v>202</v>
+      </c>
+      <c r="O84" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" t="s">
+        <v>171</v>
+      </c>
+      <c r="D85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85" t="s">
+        <v>177</v>
+      </c>
+      <c r="J85">
+        <v>69</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="M85" t="s">
+        <v>202</v>
+      </c>
+      <c r="N85" t="s">
+        <v>202</v>
+      </c>
+      <c r="O85" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>111</v>
+      </c>
+      <c r="B86" t="s">
         <v>194</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C86" t="s">
+        <v>171</v>
+      </c>
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86" t="s">
+        <v>29</v>
+      </c>
+      <c r="I86" t="s">
+        <v>177</v>
+      </c>
+      <c r="J86">
+        <v>69</v>
+      </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+      <c r="M86" t="s">
+        <v>202</v>
+      </c>
+      <c r="N86" t="s">
+        <v>202</v>
+      </c>
+      <c r="O86" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>195</v>
       </c>
-      <c r="C82" t="s">
-        <v>173</v>
-      </c>
-      <c r="D82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-      <c r="F82">
-        <v>1</v>
-      </c>
-      <c r="G82">
-        <v>1</v>
-      </c>
-      <c r="H82" t="s">
+      <c r="B87" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" t="s">
+        <v>171</v>
+      </c>
+      <c r="D87" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87" t="s">
         <v>29</v>
       </c>
-      <c r="I82" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" t="s">
-        <v>113</v>
-      </c>
-      <c r="B83" t="s">
-        <v>196</v>
-      </c>
-      <c r="C83" t="s">
-        <v>173</v>
-      </c>
-      <c r="D83" t="s">
-        <v>22</v>
-      </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="F83">
-        <v>1</v>
-      </c>
-      <c r="G83">
-        <v>1</v>
-      </c>
-      <c r="H83" t="s">
-        <v>29</v>
-      </c>
-      <c r="I83" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" t="s">
-        <v>197</v>
-      </c>
-      <c r="B84" t="s">
-        <v>198</v>
-      </c>
-      <c r="C84" t="s">
-        <v>173</v>
-      </c>
-      <c r="D84" t="s">
-        <v>106</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-      <c r="F84">
-        <v>1</v>
-      </c>
-      <c r="G84">
-        <v>1</v>
-      </c>
-      <c r="H84" t="s">
-        <v>29</v>
-      </c>
-      <c r="I84" t="s">
+      <c r="I87" t="s">
         <v>30</v>
       </c>
+      <c r="J87">
+        <v>69</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+      <c r="M87" t="s">
+        <v>202</v>
+      </c>
+      <c r="N87" t="s">
+        <v>202</v>
+      </c>
+      <c r="O87" t="s">
+        <v>202</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J75">
-    <sortCondition ref="D2:D75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
+    <sortCondition ref="D2:D78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>